<commit_message>
improved test cases, fixed shortcut test mistake
</commit_message>
<xml_diff>
--- a/Tests/integrationTests/01a_AsTeRICS_Setup/Test_cases_AsTeRICS_installation_windows.xlsx
+++ b/Tests/integrationTests/01a_AsTeRICS_Setup/Test_cases_AsTeRICS_installation_windows.xlsx
@@ -174,25 +174,6 @@
 Java 64bit: http://www.java.com/de/download/manual.jsp</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">0. Deinstall AsTeRICS if already existing
-1. Execute Setup_AsTeRICS_xxx.exe
-2. Don't choose option to include installation of embedded java
-3. Install current </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Java 8  JRE 64bit</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">1. AsTeRICS must be installed to 
 C:\Program Files (x86)\AsTeRICS
 2. ACS/ACS.exe must start without error message
@@ -250,6 +231,46 @@
     <t>Freshly installed OS without Java, .NET and Visual Studio 2010 preinstalled
 Provided Asterics Installer, or latest release candidate https://github.com/asterics/AsTeRICS/releases
 For some tests, Java is needed: http://www.java.com/de/download/manual.jsp</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">0. Deinstall AsTeRICS if already existing and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>all JRE 32-bit installations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1. Execute Setup_AsTeRICS_xxx.exe
+2. Don't choose option to include installation of embedded java
+3. Install current </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Java 8  JRE 64bit</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -636,7 +657,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -647,7 +668,7 @@
   <dimension ref="A1:F82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,7 +704,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>11</v>
@@ -717,7 +738,7 @@
     </row>
     <row r="7" spans="1:6" ht="86.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>16</v>
@@ -735,37 +756,37 @@
     </row>
     <row r="8" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="F9" s="5"/>
     </row>

</xml_diff>